<commit_message>
add in Darren suggestions
</commit_message>
<xml_diff>
--- a/keyword_thesauri.xlsx
+++ b/keyword_thesauri.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmaurer/GitHub/jrn_metadata_standards/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/JornadaFiles/LTER_IM/JRN_Metadata_Standards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29ADEA8-0B01-0049-9E0B-E63D4C09E381}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C6D221-2B57-594B-8D0E-FB81686AD764}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="14920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="393">
   <si>
     <t>Data Category</t>
   </si>
@@ -1090,9 +1090,6 @@
     <t>NEAT</t>
   </si>
   <si>
-    <t>conmod</t>
-  </si>
-  <si>
     <t>SMES</t>
   </si>
   <si>
@@ -1120,9 +1117,6 @@
     <t>Not sure how useful these placenames are</t>
   </si>
   <si>
-    <t>Defined by LTER network: Choose one</t>
-  </si>
-  <si>
     <t>Jornada Basin LTER dataset groups (length, funding cycle, subject matter): select "core" if applicable, and one or more other groups</t>
   </si>
   <si>
@@ -1136,6 +1130,81 @@
   </si>
   <si>
     <t>The LTER controlled vocabulary should be used for all data packages. Others have guidelines shown.</t>
+  </si>
+  <si>
+    <t>Conmod</t>
+  </si>
+  <si>
+    <t>Ecotone</t>
+  </si>
+  <si>
+    <t>G-SAND</t>
+  </si>
+  <si>
+    <t>G-SUMM</t>
+  </si>
+  <si>
+    <t>M-NORT</t>
+  </si>
+  <si>
+    <t>M-RABB</t>
+  </si>
+  <si>
+    <t>M-WELL</t>
+  </si>
+  <si>
+    <t>P-COLL</t>
+  </si>
+  <si>
+    <t>P-SMAL</t>
+  </si>
+  <si>
+    <t>P-TOBO</t>
+  </si>
+  <si>
+    <t>T-EAST</t>
+  </si>
+  <si>
+    <t>T-TAYL</t>
+  </si>
+  <si>
+    <t>Stressor1</t>
+  </si>
+  <si>
+    <t>Stressor2</t>
+  </si>
+  <si>
+    <t>Scrape Site</t>
+  </si>
+  <si>
+    <t>Pasture 13 burn</t>
+  </si>
+  <si>
+    <t>Gravelly Ridges</t>
+  </si>
+  <si>
+    <t>JORNEX</t>
+  </si>
+  <si>
+    <t>JRN Weatherstation</t>
+  </si>
+  <si>
+    <t>Permanent Quadrats</t>
+  </si>
+  <si>
+    <t>Tromble Watershed</t>
+  </si>
+  <si>
+    <t>HQ</t>
+  </si>
+  <si>
+    <t>JER</t>
+  </si>
+  <si>
+    <t>CDRRC</t>
+  </si>
+  <si>
+    <t>Defined by LTER network: Choose one or more</t>
   </si>
 </sst>
 </file>
@@ -1590,7 +1659,7 @@
   <dimension ref="A2:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="I9" sqref="I9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1610,17 +1679,17 @@
   <sheetData>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
@@ -1654,15 +1723,15 @@
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B9" s="12"/>
       <c r="E9" s="11" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F9" s="12"/>
       <c r="I9" s="13" t="s">
-        <v>364</v>
+        <v>392</v>
       </c>
       <c r="J9" s="14"/>
     </row>
@@ -1750,7 +1819,7 @@
       </c>
       <c r="C13" s="6"/>
       <c r="E13" s="2" t="s">
-        <v>354</v>
+        <v>368</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>350</v>
@@ -1773,7 +1842,7 @@
       </c>
       <c r="C14" s="6"/>
       <c r="E14" s="2" t="s">
-        <v>113</v>
+        <v>369</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>350</v>
@@ -1796,7 +1865,7 @@
       </c>
       <c r="C15" s="6"/>
       <c r="E15" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>350</v>
@@ -1819,13 +1888,13 @@
       </c>
       <c r="C16" s="6"/>
       <c r="E16" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>350</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>348</v>
@@ -1843,16 +1912,16 @@
         <v>351</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>350</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>349</v>
@@ -1877,7 +1946,7 @@
         <v>350</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K18" s="6"/>
     </row>
@@ -1889,16 +1958,16 @@
         <v>351</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>350</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K19" s="6"/>
     </row>
@@ -1911,13 +1980,13 @@
       </c>
       <c r="C20" s="6"/>
       <c r="E20" s="2" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>350</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K20" s="6"/>
     </row>
@@ -1929,113 +1998,251 @@
         <v>351</v>
       </c>
       <c r="C21" s="6"/>
+      <c r="E21" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G21" s="6"/>
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C22" s="6"/>
+      <c r="E22" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G22" s="6"/>
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C23" s="6"/>
+      <c r="E23" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G23" s="6"/>
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C24" s="6"/>
+      <c r="E24" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G24" s="6"/>
       <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C25" s="6"/>
+      <c r="E25" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C26" s="6"/>
+      <c r="E26" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G26" s="6"/>
       <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C27" s="6"/>
+      <c r="E27" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G27" s="6"/>
       <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C28" s="6"/>
+      <c r="E28" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G28" s="6"/>
       <c r="K28" s="6"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C29" s="6"/>
+      <c r="E29" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G29" s="6"/>
       <c r="K29" s="6"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C30" s="6"/>
+      <c r="E30" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G30" s="6"/>
       <c r="K30" s="6"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C31" s="6"/>
+      <c r="E31" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G31" s="6"/>
       <c r="K31" s="6"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C32" s="6"/>
+      <c r="E32" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G32" s="6"/>
       <c r="K32" s="6"/>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C33" s="6"/>
+      <c r="E33" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G33" s="6"/>
       <c r="K33" s="6"/>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C34" s="6"/>
+      <c r="E34" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G34" s="6"/>
       <c r="K34" s="6"/>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C35" s="6"/>
+      <c r="E35" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G35" s="6"/>
       <c r="K35" s="6"/>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C36" s="6"/>
+      <c r="E36" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G36" s="6"/>
       <c r="K36" s="6"/>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C37" s="6"/>
+      <c r="E37" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G37" s="6"/>
       <c r="K37" s="6"/>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C38" s="6"/>
+      <c r="E38" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G38" s="6"/>
       <c r="K38" s="6"/>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C39" s="6"/>
+      <c r="E39" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G39" s="6"/>
       <c r="K39" s="6"/>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C40" s="6"/>
+      <c r="E40" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G40" s="6"/>
       <c r="K40" s="6"/>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C41" s="6"/>
+      <c r="E41" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="G41" s="6"/>
       <c r="K41" s="6"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.15">
+      <c r="E42" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="K42" s="6"/>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.15">
+      <c r="E43" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>350</v>
+      </c>
       <c r="K43" s="6"/>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
new thesauri by darren
</commit_message>
<xml_diff>
--- a/keyword_thesauri.xlsx
+++ b/keyword_thesauri.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/JornadaFiles-1/LTER_IM/JRN_Metadata_Standards/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\DataProducts\LTER_IM\JRN_Metadata_Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D2F681-1CF8-8445-B3E8-AECB4C7EAC01}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="14920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="14920"/>
   </bookViews>
   <sheets>
     <sheet name="Current_Thesauri" sheetId="2" r:id="rId1"/>
     <sheet name="Old_DEIMS_Thesauri" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="400">
   <si>
     <t>Data Category</t>
   </si>
@@ -1078,15 +1077,9 @@
     <t>Human-Environment Interactions</t>
   </si>
   <si>
-    <t>Jornada Keywords</t>
-  </si>
-  <si>
     <t>JRN Dataset Keywords</t>
   </si>
   <si>
-    <t>ANPP</t>
-  </si>
-  <si>
     <t>NEAT</t>
   </si>
   <si>
@@ -1114,9 +1107,6 @@
     <t>T-WEST</t>
   </si>
   <si>
-    <t>Not sure how useful these placenames are</t>
-  </si>
-  <si>
     <t>Jornada project names and place names: choose any applicable.</t>
   </si>
   <si>
@@ -1214,13 +1204,34 @@
   </si>
   <si>
     <t>Jornada Basin LTER dataset groups (length, funding cycle, subject matter): select "core" or "non-core" , and one or more other keywords</t>
+  </si>
+  <si>
+    <t>Jornada Place Names</t>
+  </si>
+  <si>
+    <t>Jornada Project Names</t>
+  </si>
+  <si>
+    <t>NPP</t>
+  </si>
+  <si>
+    <t>NPP locations</t>
+  </si>
+  <si>
+    <t>both project and place</t>
+  </si>
+  <si>
+    <t>Pasture 9</t>
+  </si>
+  <si>
+    <t>Study XXX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1288,12 +1299,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -1346,7 +1363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1366,6 +1383,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1664,87 +1686,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="16.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="30.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="28.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="1" style="11" customWidth="1"/>
+    <col min="5" max="5" width="28.6328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="1" style="11" customWidth="1"/>
+    <col min="9" max="9" width="28.6328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1796875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="1" style="11" customWidth="1"/>
+    <col min="13" max="13" width="30.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="17.5">
       <c r="A2" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="17.5">
       <c r="A3" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="17.5">
       <c r="A4" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="3" t="s">
         <v>344</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="D6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="L6" s="12"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A8" s="15" t="s">
-        <v>351</v>
-      </c>
-      <c r="B8" s="15"/>
+      <c r="D7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="L7" s="12"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="B8" s="18"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="15" t="s">
-        <v>350</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="I8" s="16" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="18" t="s">
+        <v>393</v>
+      </c>
+      <c r="J8" s="18"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>395</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="E9" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="I9" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="N8" s="19"/>
+    </row>
+    <row r="9" spans="1:15" s="5" customFormat="1" ht="47" customHeight="1">
+      <c r="A9" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="N9" s="17"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="3" t="s">
         <v>343</v>
       </c>
@@ -1772,554 +1815,656 @@
       <c r="K10" s="3" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="M10" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="2" t="s">
         <v>347</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C11" s="6"/>
       <c r="E11" s="2" t="s">
-        <v>352</v>
+        <v>395</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>350</v>
+        <v>394</v>
       </c>
       <c r="G11" s="6"/>
       <c r="I11" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K11" s="6"/>
+      <c r="M11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="2" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C12" s="6"/>
       <c r="E12" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G12" s="6"/>
+        <v>394</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>397</v>
+      </c>
       <c r="I12" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C13" s="6"/>
       <c r="E13" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>350</v>
+        <v>394</v>
       </c>
       <c r="G13" s="6"/>
       <c r="I13" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="M13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C14" s="6"/>
       <c r="E14" s="2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>350</v>
+        <v>394</v>
       </c>
       <c r="G14" s="6"/>
       <c r="I14" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="M14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C15" s="6"/>
       <c r="E15" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G15" s="6"/>
+        <v>394</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>397</v>
+      </c>
       <c r="I15" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K15" s="6"/>
+      <c r="M15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C16" s="6"/>
       <c r="E16" s="2" t="s">
-        <v>357</v>
+        <v>376</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>350</v>
+        <v>394</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>362</v>
+        <v>397</v>
       </c>
       <c r="I16" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K16" s="6"/>
+      <c r="M16" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C17" s="6"/>
       <c r="E17" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>362</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="J17" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="M17" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>360</v>
+        <v>378</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>350</v>
+        <v>394</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>362</v>
+        <v>397</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>393</v>
       </c>
       <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C19" s="6"/>
       <c r="E19" s="2" t="s">
-        <v>359</v>
+        <v>379</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>362</v>
+        <v>394</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="I19" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>393</v>
       </c>
       <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O19" s="6"/>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>350</v>
+        <v>394</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>362</v>
+        <v>397</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>393</v>
       </c>
       <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C21" s="6"/>
       <c r="E21" s="2" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>350</v>
+        <v>394</v>
       </c>
       <c r="G21" s="6"/>
+      <c r="I21" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>393</v>
+      </c>
       <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C22" s="6"/>
       <c r="E22" s="2" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>350</v>
+        <v>394</v>
       </c>
       <c r="G22" s="6"/>
+      <c r="I22" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>393</v>
+      </c>
       <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="1:15">
       <c r="C23" s="6"/>
       <c r="E23" s="2" t="s">
-        <v>372</v>
+        <v>71</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>350</v>
+        <v>394</v>
       </c>
       <c r="G23" s="6"/>
+      <c r="I23" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>393</v>
+      </c>
       <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="1:15">
       <c r="C24" s="6"/>
       <c r="E24" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K24" s="6"/>
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="C25" s="6"/>
+      <c r="I25" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K25" s="6"/>
+      <c r="O25" s="6"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="C26" s="6"/>
+      <c r="I26" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G24" s="6"/>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="C25" s="6"/>
-      <c r="E25" s="2" t="s">
+      <c r="J26" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K26" s="6"/>
+      <c r="O26" s="6"/>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="C27" s="6"/>
+      <c r="I27" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G25" s="6"/>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="C26" s="6"/>
-      <c r="E26" s="2" t="s">
+      <c r="J27" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K27" s="6"/>
+      <c r="O27" s="6"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="C28" s="6"/>
+      <c r="I28" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G26" s="6"/>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="C27" s="6"/>
-      <c r="E27" s="2" t="s">
+      <c r="J28" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K28" s="6"/>
+      <c r="O28" s="6"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="C29" s="6"/>
+      <c r="I29" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K29" s="6"/>
+      <c r="O29" s="6"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="C30" s="6"/>
+      <c r="I30" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G27" s="6"/>
-      <c r="K27" s="6"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="C28" s="6"/>
-      <c r="E28" s="2" t="s">
+      <c r="J30" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="O30" s="6"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="C31" s="6"/>
+      <c r="I31" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G28" s="6"/>
-      <c r="K28" s="6"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="C29" s="6"/>
-      <c r="E29" s="2" t="s">
+      <c r="J31" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="O31" s="6"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="C32" s="6"/>
+      <c r="I32" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G29" s="6"/>
-      <c r="K29" s="6"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="C30" s="6"/>
-      <c r="E30" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G30" s="6"/>
-      <c r="K30" s="6"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="C31" s="6"/>
-      <c r="E31" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G31" s="6"/>
-      <c r="K31" s="6"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="C32" s="6"/>
-      <c r="E32" s="2" t="s">
+      <c r="J32" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="O32" s="6"/>
+    </row>
+    <row r="33" spans="3:15">
+      <c r="C33" s="6"/>
+      <c r="I33" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G32" s="6"/>
-      <c r="K32" s="6"/>
-    </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="C33" s="6"/>
-      <c r="E33" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G33" s="6"/>
-      <c r="K33" s="6"/>
-    </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.15">
+      <c r="J33" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="O33" s="6"/>
+    </row>
+    <row r="34" spans="3:15">
       <c r="C34" s="6"/>
-      <c r="E34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G34" s="6"/>
+      <c r="J34" s="2" t="s">
+        <v>393</v>
+      </c>
       <c r="K34" s="6"/>
-    </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.15">
+      <c r="O34" s="6"/>
+    </row>
+    <row r="35" spans="3:15">
       <c r="C35" s="6"/>
-      <c r="E35" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G35" s="6"/>
+      <c r="I35" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>393</v>
+      </c>
       <c r="K35" s="6"/>
-    </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.15">
+      <c r="O35" s="6"/>
+    </row>
+    <row r="36" spans="3:15">
       <c r="C36" s="6"/>
-      <c r="E36" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G36" s="6"/>
+      <c r="I36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>393</v>
+      </c>
       <c r="K36" s="6"/>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.15">
+      <c r="O36" s="6"/>
+    </row>
+    <row r="37" spans="3:15">
       <c r="C37" s="6"/>
-      <c r="E37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G37" s="6"/>
+      <c r="J37" s="2" t="s">
+        <v>393</v>
+      </c>
       <c r="K37" s="6"/>
-    </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.15">
+      <c r="O37" s="6"/>
+    </row>
+    <row r="38" spans="3:15">
       <c r="C38" s="6"/>
-      <c r="E38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G38" s="6"/>
+      <c r="J38" s="2" t="s">
+        <v>393</v>
+      </c>
       <c r="K38" s="6"/>
-    </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.15">
+      <c r="O38" s="6"/>
+    </row>
+    <row r="39" spans="3:15">
       <c r="C39" s="6"/>
-      <c r="E39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G39" s="6"/>
+      <c r="J39" s="2" t="s">
+        <v>393</v>
+      </c>
       <c r="K39" s="6"/>
-    </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.15">
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="3:15">
       <c r="C40" s="6"/>
-      <c r="E40" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G40" s="6"/>
-      <c r="K40" s="6"/>
-    </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.15">
+      <c r="I40" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="O40" s="6"/>
+    </row>
+    <row r="41" spans="3:15">
       <c r="C41" s="6"/>
-      <c r="E41" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G41" s="6"/>
-      <c r="K41" s="6"/>
-    </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="E42" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="K42" s="6"/>
-    </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="E43" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="K43" s="6"/>
-    </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="E44" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="K44" s="6"/>
-    </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="E45" s="2" t="s">
+      <c r="J41" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="K45" s="6"/>
-    </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="K46" s="6"/>
-    </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.15">
-      <c r="K47" s="6"/>
+      <c r="O41" s="6"/>
+    </row>
+    <row r="42" spans="3:15">
+      <c r="I42" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="O42" s="6"/>
+    </row>
+    <row r="43" spans="3:15">
+      <c r="O43" s="6"/>
+    </row>
+    <row r="44" spans="3:15">
+      <c r="O44" s="6"/>
+    </row>
+    <row r="45" spans="3:15">
+      <c r="O45" s="6"/>
+    </row>
+    <row r="46" spans="3:15">
+      <c r="O46" s="6"/>
+    </row>
+    <row r="47" spans="3:15">
+      <c r="O47" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="M9:N9"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="M8:N8"/>
     <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T305"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.1640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="23.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" style="2" customWidth="1"/>
+    <col min="3" max="4" width="23.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" style="2" customWidth="1"/>
     <col min="6" max="6" width="15" style="2" customWidth="1"/>
-    <col min="7" max="7" width="33.6640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="2"/>
+    <col min="7" max="7" width="33.6328125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2342,7 +2487,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2365,7 +2510,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2388,7 +2533,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2405,7 +2550,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2422,7 +2567,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2439,7 +2584,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2453,7 +2598,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2467,7 +2612,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2478,7 +2623,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2489,7 +2634,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7">
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
@@ -2497,1194 +2642,1194 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7">
       <c r="G12" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7">
       <c r="G13" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7">
       <c r="G14" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7">
       <c r="G15" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7">
       <c r="G16" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="7:11">
       <c r="G17" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="7:11">
       <c r="G18" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="7:11">
       <c r="G19" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="7:11">
       <c r="G20" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="7:11">
       <c r="G21" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="7:11">
       <c r="G22" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="7:11">
       <c r="G23" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="7:11">
       <c r="G24" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="7:11">
       <c r="G25" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="7:11">
       <c r="G26" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="7:11">
       <c r="G27" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="7:11">
       <c r="G28" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="7:11">
       <c r="G29" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="7:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="7:11" ht="15.5">
       <c r="G30" s="2" t="s">
         <v>324</v>
       </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="7:11">
       <c r="G31" s="2" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="32" spans="7:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="7:11">
       <c r="G32" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="33" spans="7:20">
       <c r="G33" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="34" spans="7:20">
       <c r="G34" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="35" spans="7:20">
       <c r="G35" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="36" spans="7:20">
       <c r="G36" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="37" spans="7:20">
       <c r="G37" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="38" spans="7:20">
       <c r="G38" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="39" spans="7:20">
       <c r="G39" s="2" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="40" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="40" spans="7:20">
       <c r="G40" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="41" spans="7:20">
       <c r="G41" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="7:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="7:20" ht="15.5">
       <c r="G42" s="2" t="s">
         <v>77</v>
       </c>
       <c r="T42" s="10"/>
     </row>
-    <row r="43" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="43" spans="7:20">
       <c r="G43" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="44" spans="7:20">
       <c r="G44" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="45" spans="7:20">
       <c r="G45" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="46" spans="7:20">
       <c r="G46" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="47" spans="7:20">
       <c r="G47" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="7:20" x14ac:dyDescent="0.15">
+    <row r="48" spans="7:20">
       <c r="G48" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="49" spans="7:7">
       <c r="G49" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="50" spans="7:7">
       <c r="G50" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="51" spans="7:7">
       <c r="G51" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="52" spans="7:7">
       <c r="G52" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="53" spans="7:7">
       <c r="G53" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="54" spans="7:7">
       <c r="G54" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="55" spans="7:7">
       <c r="G55" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="56" spans="7:7">
       <c r="G56" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="57" spans="7:7">
       <c r="G57" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="58" spans="7:7">
       <c r="G58" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="59" spans="7:7">
       <c r="G59" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="60" spans="7:7">
       <c r="G60" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="61" spans="7:7">
       <c r="G61" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="62" spans="7:7">
       <c r="G62" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="63" spans="7:7">
       <c r="G63" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="64" spans="7:7">
       <c r="G64" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="65" spans="7:7">
       <c r="G65" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="66" spans="7:7">
       <c r="G66" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="67" spans="7:7">
       <c r="G67" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="68" spans="7:7">
       <c r="G68" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="69" spans="7:7">
       <c r="G69" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="70" spans="7:7">
       <c r="G70" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="71" spans="7:7">
       <c r="G71" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="72" spans="7:7">
       <c r="G72" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="73" spans="7:7">
       <c r="G73" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="74" spans="7:7">
       <c r="G74" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="75" spans="7:7">
       <c r="G75" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="76" spans="7:7">
       <c r="G76" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="77" spans="7:7">
       <c r="G77" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="78" spans="7:7">
       <c r="G78" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="79" spans="7:7">
       <c r="G79" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="80" spans="7:7">
       <c r="G80" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="81" spans="7:7">
       <c r="G81" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="82" spans="7:7">
       <c r="G82" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="83" spans="7:7">
       <c r="G83" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="84" spans="7:7">
       <c r="G84" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="85" spans="7:7">
       <c r="G85" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="86" spans="7:7">
       <c r="G86" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="87" spans="7:7">
       <c r="G87" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="88" spans="7:7">
       <c r="G88" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="89" spans="7:7">
       <c r="G89" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="90" spans="7:7">
       <c r="G90" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="91" spans="7:7">
       <c r="G91" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="92" spans="7:7">
       <c r="G92" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="93" spans="7:7">
       <c r="G93" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="94" spans="7:7">
       <c r="G94" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="95" spans="7:7">
       <c r="G95" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="96" spans="7:7">
       <c r="G96" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="97" spans="7:7">
       <c r="G97" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="98" spans="7:7">
       <c r="G98" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="99" spans="7:7">
       <c r="G99" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="100" spans="7:7">
       <c r="G100" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="101" spans="7:7">
       <c r="G101" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="102" spans="7:7">
       <c r="G102" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="103" spans="7:7">
       <c r="G103" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="104" spans="7:7">
       <c r="G104" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="105" spans="7:7">
       <c r="G105" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="106" spans="7:7">
       <c r="G106" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="107" spans="7:7">
       <c r="G107" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="108" spans="7:7">
       <c r="G108" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="109" spans="7:7">
       <c r="G109" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="110" spans="7:7">
       <c r="G110" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="111" spans="7:7">
       <c r="G111" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="112" spans="7:7">
       <c r="G112" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="113" spans="7:7">
       <c r="G113" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="114" spans="7:7">
       <c r="G114" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="115" spans="7:7">
       <c r="G115" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="116" spans="7:7">
       <c r="G116" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="117" spans="7:7">
       <c r="G117" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="118" spans="7:7">
       <c r="G118" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="119" spans="7:7">
       <c r="G119" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="120" spans="7:7">
       <c r="G120" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="121" spans="7:7">
       <c r="G121" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="122" spans="7:7">
       <c r="G122" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="123" spans="7:7">
       <c r="G123" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="124" spans="7:7">
       <c r="G124" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="125" spans="7:7">
       <c r="G125" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="126" spans="7:7">
       <c r="G126" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="127" spans="7:7">
       <c r="G127" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="128" spans="7:7">
       <c r="G128" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="129" spans="7:7">
       <c r="G129" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="130" spans="7:7">
       <c r="G130" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="131" spans="7:7">
       <c r="G131" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="132" spans="7:7">
       <c r="G132" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="133" spans="7:7">
       <c r="G133" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="134" spans="7:7">
       <c r="G134" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="135" spans="7:7">
       <c r="G135" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="136" spans="7:7">
       <c r="G136" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="137" spans="7:7">
       <c r="G137" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="138" spans="7:7">
       <c r="G138" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="139" spans="7:7">
       <c r="G139" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="140" spans="7:7">
       <c r="G140" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="141" spans="7:7">
       <c r="G141" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="142" spans="7:7">
       <c r="G142" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="143" spans="7:7">
       <c r="G143" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="144" spans="7:7">
       <c r="G144" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="145" spans="7:7">
       <c r="G145" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="146" spans="7:7">
       <c r="G146" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="147" spans="7:7">
       <c r="G147" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="148" spans="7:7">
       <c r="G148" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="149" spans="7:7">
       <c r="G149" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="150" spans="7:7">
       <c r="G150" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="151" spans="7:7">
       <c r="G151" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="152" spans="7:7">
       <c r="G152" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="153" spans="7:7">
       <c r="G153" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="154" spans="7:7">
       <c r="G154" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="155" spans="7:7">
       <c r="G155" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="156" spans="7:7">
       <c r="G156" s="2" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="157" spans="7:7">
       <c r="G157" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="158" spans="7:7">
       <c r="G158" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="159" spans="7:7">
       <c r="G159" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="160" spans="7:7">
       <c r="G160" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="161" spans="7:7">
       <c r="G161" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="162" spans="7:7">
       <c r="G162" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="163" spans="7:7">
       <c r="G163" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="164" spans="7:7">
       <c r="G164" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="165" spans="7:7">
       <c r="G165" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="166" spans="7:7">
       <c r="G166" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="167" spans="7:7">
       <c r="G167" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="168" spans="7:7">
       <c r="G168" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="169" spans="7:7">
       <c r="G169" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="170" spans="7:7">
       <c r="G170" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="171" spans="7:7">
       <c r="G171" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="172" spans="7:7">
       <c r="G172" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="173" spans="7:7">
       <c r="G173" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="174" spans="7:7">
       <c r="G174" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="175" spans="7:7">
       <c r="G175" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="176" spans="7:7">
       <c r="G176" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="177" spans="7:7">
       <c r="G177" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="178" spans="7:7">
       <c r="G178" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="179" spans="7:7">
       <c r="G179" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="180" spans="7:7">
       <c r="G180" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="181" spans="7:7">
       <c r="G181" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="182" spans="7:7">
       <c r="G182" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="183" spans="7:7">
       <c r="G183" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="184" spans="7:7">
       <c r="G184" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="185" spans="7:7">
       <c r="G185" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="186" spans="7:7">
       <c r="G186" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="187" spans="7:7">
       <c r="G187" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="188" spans="7:7">
       <c r="G188" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="189" spans="7:7">
       <c r="G189" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="190" spans="7:7">
       <c r="G190" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="191" spans="7:7">
       <c r="G191" s="2" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="192" spans="7:7">
       <c r="G192" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="193" spans="7:7">
       <c r="G193" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="194" spans="7:7">
       <c r="G194" s="2" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="195" spans="7:7">
       <c r="G195" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="196" spans="7:7">
       <c r="G196" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="197" spans="7:7">
       <c r="G197" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="198" spans="7:7">
       <c r="G198" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="199" spans="7:7">
       <c r="G199" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="200" spans="7:7">
       <c r="G200" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="201" spans="7:7">
       <c r="G201" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="202" spans="7:7">
       <c r="G202" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="203" spans="7:7">
       <c r="G203" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="204" spans="7:7">
       <c r="G204" s="2" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="205" spans="7:7">
       <c r="G205" s="2" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="206" spans="7:7">
       <c r="G206" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="207" spans="7:7">
       <c r="G207" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="208" spans="7:7">
       <c r="G208" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="209" spans="7:7">
       <c r="G209" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="210" spans="7:7">
       <c r="G210" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="211" spans="7:7">
       <c r="G211" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="212" spans="7:7">
       <c r="G212" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="213" spans="7:7">
       <c r="G213" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="214" spans="7:7">
       <c r="G214" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="215" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="215" spans="7:7">
       <c r="G215" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="216" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="216" spans="7:7">
       <c r="G216" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="217" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="217" spans="7:7">
       <c r="G217" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="218" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="218" spans="7:7">
       <c r="G218" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="219" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="219" spans="7:7">
       <c r="G219" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="220" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="220" spans="7:7">
       <c r="G220" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="221" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="221" spans="7:7">
       <c r="G221" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="222" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="222" spans="7:7">
       <c r="G222" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="223" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="223" spans="7:7">
       <c r="G223" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="224" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="224" spans="7:7">
       <c r="G224" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="225" spans="7:7">
       <c r="G225" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="226" spans="7:7">
       <c r="G226" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="227" spans="7:7">
       <c r="G227" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="228" spans="7:7">
       <c r="G228" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="229" spans="7:7">
       <c r="G229" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="230" spans="7:7">
       <c r="G230" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="231" spans="7:7">
       <c r="G231" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="232" spans="7:7">
       <c r="G232" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="233" spans="7:7">
       <c r="G233" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="234" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="234" spans="7:7">
       <c r="G234" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="235" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="235" spans="7:7">
       <c r="G235" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="236" spans="7:7">
       <c r="G236" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="237" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="237" spans="7:7">
       <c r="G237" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="238" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="238" spans="7:7">
       <c r="G238" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="239" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="239" spans="7:7">
       <c r="G239" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="240" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="240" spans="7:7">
       <c r="G240" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="241" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="241" spans="7:8">
       <c r="G241" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="242" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="242" spans="7:8">
       <c r="G242" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="243" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="243" spans="7:8">
       <c r="G243" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="244" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="244" spans="7:8">
       <c r="G244" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="245" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="245" spans="7:8">
       <c r="G245" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="246" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="246" spans="7:8">
       <c r="G246" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="247" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="247" spans="7:8">
       <c r="G247" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="248" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="248" spans="7:8">
       <c r="G248" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="249" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="249" spans="7:8">
       <c r="G249" s="2" t="s">
         <v>270</v>
       </c>
@@ -3692,288 +3837,288 @@
         <v>271</v>
       </c>
     </row>
-    <row r="250" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="250" spans="7:8">
       <c r="G250" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="251" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="251" spans="7:8">
       <c r="G251" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="252" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="252" spans="7:8">
       <c r="G252" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="253" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="253" spans="7:8">
       <c r="G253" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="254" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="254" spans="7:8">
       <c r="G254" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="255" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="255" spans="7:8">
       <c r="G255" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="256" spans="7:8" x14ac:dyDescent="0.15">
+    <row r="256" spans="7:8">
       <c r="G256" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="257" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="257" spans="7:7">
       <c r="G257" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="258" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="258" spans="7:7">
       <c r="G258" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="259" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="259" spans="7:7">
       <c r="G259" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="260" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="260" spans="7:7">
       <c r="G260" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="261" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="261" spans="7:7">
       <c r="G261" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="262" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="262" spans="7:7">
       <c r="G262" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="263" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="263" spans="7:7">
       <c r="G263" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="264" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="264" spans="7:7">
       <c r="G264" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="265" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="265" spans="7:7">
       <c r="G265" s="2" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="266" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="266" spans="7:7">
       <c r="G266" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="267" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="267" spans="7:7">
       <c r="G267" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="268" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="268" spans="7:7">
       <c r="G268" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="269" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="269" spans="7:7">
       <c r="G269" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="270" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="270" spans="7:7">
       <c r="G270" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="271" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="271" spans="7:7">
       <c r="G271" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="272" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="272" spans="7:7">
       <c r="G272" s="2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="273" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="273" spans="7:7">
       <c r="G273" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="274" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="274" spans="7:7">
       <c r="G274" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="275" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="275" spans="7:7">
       <c r="G275" s="2" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="276" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="276" spans="7:7">
       <c r="G276" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="277" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="277" spans="7:7">
       <c r="G277" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="278" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="278" spans="7:7">
       <c r="G278" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="279" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="279" spans="7:7">
       <c r="G279" s="2" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="280" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="280" spans="7:7">
       <c r="G280" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="281" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="281" spans="7:7">
       <c r="G281" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="282" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="282" spans="7:7">
       <c r="G282" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="283" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="283" spans="7:7">
       <c r="G283" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="284" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="284" spans="7:7">
       <c r="G284" s="2" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="285" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="285" spans="7:7">
       <c r="G285" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="286" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="286" spans="7:7">
       <c r="G286" s="2" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="287" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="287" spans="7:7">
       <c r="G287" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="288" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="288" spans="7:7">
       <c r="G288" s="2" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="289" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="289" spans="7:7">
       <c r="G289" s="2" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="290" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="290" spans="7:7">
       <c r="G290" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="291" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="291" spans="7:7">
       <c r="G291" s="2" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="292" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="292" spans="7:7">
       <c r="G292" s="2" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="293" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="293" spans="7:7">
       <c r="G293" s="2" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="294" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="294" spans="7:7">
       <c r="G294" s="2" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="295" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="295" spans="7:7">
       <c r="G295" s="2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="296" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="296" spans="7:7">
       <c r="G296" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="297" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="297" spans="7:7">
       <c r="G297" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="298" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="298" spans="7:7">
       <c r="G298" s="2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="299" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="299" spans="7:7">
       <c r="G299" s="2" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="300" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="300" spans="7:7">
       <c r="G300" s="2" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="301" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="301" spans="7:7">
       <c r="G301" s="2" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="302" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="302" spans="7:7">
       <c r="G302" s="2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="303" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="303" spans="7:7">
       <c r="G303" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="304" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="304" spans="7:7">
       <c r="G304" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="305" spans="7:7" x14ac:dyDescent="0.15">
+    <row r="305" spans="7:7">
       <c r="G305" s="2" t="s">
         <v>323</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H305">
+  <sortState ref="A2:H305">
     <sortCondition ref="G2:G305"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed G-SAND keyword to G-IBPE
* Key words for this in data packages will need to be changed
* Keyword templates for most NPP packages changed, but verify and publish
</commit_message>
<xml_diff>
--- a/keyword_thesauri.xlsx
+++ b/keyword_thesauri.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\DataProducts\LTER_IM\JRN_Metadata_Standards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataProducts/LTER_IM/JRN_Metadata_Standards/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F04702-0B99-E848-AEA2-5B653AEE65AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current_Thesauri" sheetId="2" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="415">
   <si>
     <t>Data Category</t>
   </si>
@@ -1122,9 +1123,6 @@
     <t>Ecotone</t>
   </si>
   <si>
-    <t>G-SAND</t>
-  </si>
-  <si>
     <t>G-SUMM</t>
   </si>
   <si>
@@ -1215,9 +1213,6 @@
     <t>Pasture 9</t>
   </si>
   <si>
-    <t>Study XXX</t>
-  </si>
-  <si>
     <t>These are the 5 keyword thesauri available for Jornada Basin LTER data packages.</t>
   </si>
   <si>
@@ -1267,13 +1262,22 @@
   </si>
   <si>
     <t>LTER-I Transect</t>
+  </si>
+  <si>
+    <t>study XXX</t>
+  </si>
+  <si>
+    <t>G-IBPE</t>
+  </si>
+  <si>
+    <t>Was G-SAND. Pretty sure that was wrong. Making sure NPP data packages are changed…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1728,48 +1732,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="28.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="1" style="11" customWidth="1"/>
-    <col min="5" max="5" width="28.6328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="1" style="11" customWidth="1"/>
-    <col min="9" max="9" width="28.6328125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="20.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1796875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="1" style="11" customWidth="1"/>
-    <col min="13" max="13" width="30.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.81640625" style="2"/>
+    <col min="13" max="13" width="30.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="17.5">
+    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="17.5">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="17.5">
+    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>344</v>
       </c>
@@ -1780,13 +1784,13 @@
       <c r="H6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="C7" s="4"/>
       <c r="D7" s="12"/>
       <c r="H7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>350</v>
       </c>
@@ -1794,12 +1798,12 @@
       <c r="C8" s="4"/>
       <c r="D8" s="12"/>
       <c r="E8" s="18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F8" s="18"/>
       <c r="H8" s="12"/>
       <c r="I8" s="18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J8" s="18"/>
       <c r="L8" s="12"/>
@@ -1808,9 +1812,9 @@
       </c>
       <c r="N8" s="19"/>
     </row>
-    <row r="9" spans="1:15" s="5" customFormat="1" ht="47" customHeight="1">
+    <row r="9" spans="1:15" s="5" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B9" s="15"/>
       <c r="D9" s="13"/>
@@ -1825,11 +1829,11 @@
       <c r="J9" s="15"/>
       <c r="L9" s="13"/>
       <c r="M9" s="16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="N9" s="17"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>343</v>
       </c>
@@ -1867,7 +1871,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>347</v>
       </c>
@@ -1875,20 +1879,20 @@
         <v>350</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G11" s="6"/>
       <c r="I11" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K11" s="6"/>
       <c r="M11" s="2" t="s">
@@ -1899,33 +1903,33 @@
       </c>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>350</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>351</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>351</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>22</v>
@@ -1935,7 +1939,7 @@
       </c>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1947,14 +1951,14 @@
         <v>363</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G13" s="6"/>
       <c r="I13" s="2" t="s">
         <v>363</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K13" s="6"/>
       <c r="M13" s="2" t="s">
@@ -1965,7 +1969,7 @@
       </c>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1977,17 +1981,17 @@
         <v>364</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G14" s="6"/>
       <c r="I14" s="2" t="s">
         <v>352</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>24</v>
@@ -1997,7 +2001,7 @@
       </c>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2009,16 +2013,16 @@
         <v>352</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>355</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K15" s="6"/>
       <c r="M15" s="2" t="s">
@@ -2029,7 +2033,7 @@
       </c>
       <c r="O15" s="6"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2038,19 +2042,19 @@
       </c>
       <c r="C16" s="6"/>
       <c r="E16" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>356</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K16" s="6"/>
       <c r="M16" s="2" t="s">
@@ -2061,7 +2065,7 @@
       </c>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -2070,19 +2074,19 @@
       </c>
       <c r="C17" s="6"/>
       <c r="E17" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>358</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K17" s="6"/>
       <c r="M17" s="2" t="s">
@@ -2093,7 +2097,7 @@
       </c>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -2104,24 +2108,24 @@
         <v>353</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>357</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K18" s="6"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
@@ -2130,22 +2134,24 @@
       </c>
       <c r="C19" s="6"/>
       <c r="E19" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G19" s="6"/>
       <c r="I19" s="2" t="s">
-        <v>365</v>
+        <v>413</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="K19" s="6"/>
+        <v>389</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>414</v>
+      </c>
       <c r="O19" s="6"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -2156,24 +2162,24 @@
         <v>354</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K20" s="6"/>
       <c r="O20" s="6"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -2182,22 +2188,22 @@
       </c>
       <c r="C21" s="6"/>
       <c r="E21" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G21" s="6"/>
       <c r="I21" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K21" s="6"/>
       <c r="O21" s="6"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -2206,186 +2212,186 @@
       </c>
       <c r="C22" s="6"/>
       <c r="E22" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G22" s="6"/>
       <c r="I22" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K22" s="6"/>
       <c r="O22" s="6"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>350</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G23" s="6"/>
       <c r="I23" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K23" s="6"/>
       <c r="O23" s="6"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>350</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>396</v>
+        <v>412</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K24" s="6"/>
       <c r="O24" s="6"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>350</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K25" s="6"/>
       <c r="O25" s="6"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>350</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K26" s="6"/>
       <c r="O26" s="6"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>350</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>413</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K27" s="6"/>
       <c r="O27" s="6"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>350</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K28" s="6"/>
       <c r="O28" s="6"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>350</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>359</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K29" s="6"/>
       <c r="O29" s="6"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
@@ -2393,41 +2399,41 @@
         <v>350</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="O30" s="6"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>350</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="O31" s="6"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>34</v>
       </c>
@@ -2435,148 +2441,148 @@
         <v>350</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="O32" s="6"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>350</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="O33" s="6"/>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="C34" s="6"/>
       <c r="I34" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K34" s="6"/>
       <c r="O34" s="6"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="C35" s="6"/>
       <c r="I35" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K35" s="6"/>
       <c r="O35" s="6"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="C36" s="6"/>
       <c r="I36" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K36" s="6"/>
       <c r="O36" s="6"/>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="C37" s="6"/>
       <c r="I37" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K37" s="6"/>
       <c r="O37" s="6"/>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
       <c r="C38" s="6"/>
       <c r="I38" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K38" s="6"/>
       <c r="O38" s="6"/>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
       <c r="C39" s="6"/>
       <c r="I39" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K39" s="6"/>
       <c r="O39" s="6"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
       <c r="C40" s="6"/>
       <c r="I40" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="J40" s="2" t="s">
-        <v>390</v>
-      </c>
       <c r="O40" s="6"/>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="C41" s="6"/>
       <c r="I41" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="O41" s="6"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
       <c r="I42" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="O42" s="6"/>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="O43" s="6"/>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="O44" s="6"/>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
       <c r="O45" s="6"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
       <c r="O46" s="6"/>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="O47" s="6"/>
     </row>
   </sheetData>
@@ -2591,32 +2597,32 @@
     <mergeCell ref="I9:J9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T305"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.1796875" style="2" customWidth="1"/>
-    <col min="3" max="4" width="23.1796875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="23.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="15" style="2" customWidth="1"/>
-    <col min="7" max="7" width="33.6328125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.81640625" style="2"/>
+    <col min="7" max="7" width="33.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -2662,7 +2668,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2685,7 +2691,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -2702,7 +2708,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2719,7 +2725,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2736,7 +2742,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -2750,7 +2756,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2764,7 +2770,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -2775,7 +2781,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -2786,7 +2792,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
@@ -2794,1194 +2800,1194 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="G12" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="G13" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="G14" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="G15" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="G16" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="7:11">
+    <row r="17" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G17" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="7:11">
+    <row r="18" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G18" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="7:11">
+    <row r="19" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G19" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="7:11">
+    <row r="20" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G20" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="7:11">
+    <row r="21" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G21" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="7:11">
+    <row r="22" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G22" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="7:11">
+    <row r="23" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G23" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="7:11">
+    <row r="24" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G24" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="7:11">
+    <row r="25" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G25" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="7:11">
+    <row r="26" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G26" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="7:11">
+    <row r="27" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G27" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="7:11">
+    <row r="28" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G28" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="7:11">
+    <row r="29" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G29" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="7:11" ht="15.5">
+    <row r="30" spans="7:11" ht="16" x14ac:dyDescent="0.2">
       <c r="G30" s="2" t="s">
         <v>324</v>
       </c>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="7:11">
+    <row r="31" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G31" s="2" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="32" spans="7:11">
+    <row r="32" spans="7:11" x14ac:dyDescent="0.15">
       <c r="G32" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="7:20">
+    <row r="33" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G33" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="7:20">
+    <row r="34" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G34" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="7:20">
+    <row r="35" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G35" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="7:20">
+    <row r="36" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G36" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="7:20">
+    <row r="37" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G37" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="7:20">
+    <row r="38" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G38" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="7:20">
+    <row r="39" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G39" s="2" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="40" spans="7:20">
+    <row r="40" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G40" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="7:20">
+    <row r="41" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G41" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="7:20" ht="15.5">
+    <row r="42" spans="7:20" ht="16" x14ac:dyDescent="0.2">
       <c r="G42" s="2" t="s">
         <v>77</v>
       </c>
       <c r="T42" s="10"/>
     </row>
-    <row r="43" spans="7:20">
+    <row r="43" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G43" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="7:20">
+    <row r="44" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G44" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="7:20">
+    <row r="45" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G45" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="7:20">
+    <row r="46" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G46" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="7:20">
+    <row r="47" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G47" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="7:20">
+    <row r="48" spans="7:20" x14ac:dyDescent="0.15">
       <c r="G48" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="7:7">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G49" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="7:7">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G50" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="7:7">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G51" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="7:7">
+    <row r="52" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G52" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="7:7">
+    <row r="53" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G53" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="54" spans="7:7">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G54" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="7:7">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G55" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="7:7">
+    <row r="56" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G56" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="7:7">
+    <row r="57" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G57" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="7:7">
+    <row r="58" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G58" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="7:7">
+    <row r="59" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G59" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="7:7">
+    <row r="60" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G60" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="61" spans="7:7">
+    <row r="61" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G61" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="7:7">
+    <row r="62" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G62" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="63" spans="7:7">
+    <row r="63" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G63" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="64" spans="7:7">
+    <row r="64" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G64" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="7:7">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G65" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="7:7">
+    <row r="66" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G66" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="7:7">
+    <row r="67" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G67" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="7:7">
+    <row r="68" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G68" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="7:7">
+    <row r="69" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G69" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="70" spans="7:7">
+    <row r="70" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G70" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="7:7">
+    <row r="71" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G71" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="7:7">
+    <row r="72" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G72" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="73" spans="7:7">
+    <row r="73" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G73" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="7:7">
+    <row r="74" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G74" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="75" spans="7:7">
+    <row r="75" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G75" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="76" spans="7:7">
+    <row r="76" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G76" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="77" spans="7:7">
+    <row r="77" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G77" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="78" spans="7:7">
+    <row r="78" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G78" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="79" spans="7:7">
+    <row r="79" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G79" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="80" spans="7:7">
+    <row r="80" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G80" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="81" spans="7:7">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G81" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="82" spans="7:7">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G82" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="83" spans="7:7">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G83" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="84" spans="7:7">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G84" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="7:7">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G85" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="86" spans="7:7">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G86" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="87" spans="7:7">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G87" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="88" spans="7:7">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G88" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="89" spans="7:7">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G89" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="90" spans="7:7">
+    <row r="90" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G90" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="91" spans="7:7">
+    <row r="91" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G91" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="92" spans="7:7">
+    <row r="92" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G92" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="93" spans="7:7">
+    <row r="93" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G93" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="94" spans="7:7">
+    <row r="94" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G94" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="95" spans="7:7">
+    <row r="95" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G95" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="96" spans="7:7">
+    <row r="96" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G96" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="97" spans="7:7">
+    <row r="97" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G97" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="98" spans="7:7">
+    <row r="98" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G98" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="99" spans="7:7">
+    <row r="99" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G99" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="100" spans="7:7">
+    <row r="100" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G100" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="101" spans="7:7">
+    <row r="101" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G101" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="102" spans="7:7">
+    <row r="102" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G102" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="103" spans="7:7">
+    <row r="103" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G103" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="104" spans="7:7">
+    <row r="104" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G104" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="105" spans="7:7">
+    <row r="105" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G105" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="106" spans="7:7">
+    <row r="106" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G106" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="107" spans="7:7">
+    <row r="107" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G107" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="7:7">
+    <row r="108" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G108" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="109" spans="7:7">
+    <row r="109" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G109" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="110" spans="7:7">
+    <row r="110" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G110" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="111" spans="7:7">
+    <row r="111" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G111" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="112" spans="7:7">
+    <row r="112" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G112" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="113" spans="7:7">
+    <row r="113" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G113" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="7:7">
+    <row r="114" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G114" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="115" spans="7:7">
+    <row r="115" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G115" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="116" spans="7:7">
+    <row r="116" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G116" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="117" spans="7:7">
+    <row r="117" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G117" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="118" spans="7:7">
+    <row r="118" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G118" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="119" spans="7:7">
+    <row r="119" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G119" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="120" spans="7:7">
+    <row r="120" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G120" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="121" spans="7:7">
+    <row r="121" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G121" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="122" spans="7:7">
+    <row r="122" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G122" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="123" spans="7:7">
+    <row r="123" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G123" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="124" spans="7:7">
+    <row r="124" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G124" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="125" spans="7:7">
+    <row r="125" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G125" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="126" spans="7:7">
+    <row r="126" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G126" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="127" spans="7:7">
+    <row r="127" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G127" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="128" spans="7:7">
+    <row r="128" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G128" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="129" spans="7:7">
+    <row r="129" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G129" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="130" spans="7:7">
+    <row r="130" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G130" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="131" spans="7:7">
+    <row r="131" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G131" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="132" spans="7:7">
+    <row r="132" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G132" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="133" spans="7:7">
+    <row r="133" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G133" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="134" spans="7:7">
+    <row r="134" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G134" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="135" spans="7:7">
+    <row r="135" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G135" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="136" spans="7:7">
+    <row r="136" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G136" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="137" spans="7:7">
+    <row r="137" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G137" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="138" spans="7:7">
+    <row r="138" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G138" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="139" spans="7:7">
+    <row r="139" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G139" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="140" spans="7:7">
+    <row r="140" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G140" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="141" spans="7:7">
+    <row r="141" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G141" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="142" spans="7:7">
+    <row r="142" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G142" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="143" spans="7:7">
+    <row r="143" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G143" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="144" spans="7:7">
+    <row r="144" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G144" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="145" spans="7:7">
+    <row r="145" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G145" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="146" spans="7:7">
+    <row r="146" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G146" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="147" spans="7:7">
+    <row r="147" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G147" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="148" spans="7:7">
+    <row r="148" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G148" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="149" spans="7:7">
+    <row r="149" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G149" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="150" spans="7:7">
+    <row r="150" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G150" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="151" spans="7:7">
+    <row r="151" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G151" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="152" spans="7:7">
+    <row r="152" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G152" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="153" spans="7:7">
+    <row r="153" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G153" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="154" spans="7:7">
+    <row r="154" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G154" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="155" spans="7:7">
+    <row r="155" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G155" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="156" spans="7:7">
+    <row r="156" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G156" s="2" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="157" spans="7:7">
+    <row r="157" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G157" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="158" spans="7:7">
+    <row r="158" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G158" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="159" spans="7:7">
+    <row r="159" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G159" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="160" spans="7:7">
+    <row r="160" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G160" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="161" spans="7:7">
+    <row r="161" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G161" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="162" spans="7:7">
+    <row r="162" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G162" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="163" spans="7:7">
+    <row r="163" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G163" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="164" spans="7:7">
+    <row r="164" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G164" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="165" spans="7:7">
+    <row r="165" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G165" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="166" spans="7:7">
+    <row r="166" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G166" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="167" spans="7:7">
+    <row r="167" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G167" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="168" spans="7:7">
+    <row r="168" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G168" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="169" spans="7:7">
+    <row r="169" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G169" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="170" spans="7:7">
+    <row r="170" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G170" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="171" spans="7:7">
+    <row r="171" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G171" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="172" spans="7:7">
+    <row r="172" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G172" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="173" spans="7:7">
+    <row r="173" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G173" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="174" spans="7:7">
+    <row r="174" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G174" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="175" spans="7:7">
+    <row r="175" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G175" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="176" spans="7:7">
+    <row r="176" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G176" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="177" spans="7:7">
+    <row r="177" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G177" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="178" spans="7:7">
+    <row r="178" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G178" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="179" spans="7:7">
+    <row r="179" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G179" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="180" spans="7:7">
+    <row r="180" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G180" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="181" spans="7:7">
+    <row r="181" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G181" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="182" spans="7:7">
+    <row r="182" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G182" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="183" spans="7:7">
+    <row r="183" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G183" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="184" spans="7:7">
+    <row r="184" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G184" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="185" spans="7:7">
+    <row r="185" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G185" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="186" spans="7:7">
+    <row r="186" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G186" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="187" spans="7:7">
+    <row r="187" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G187" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="188" spans="7:7">
+    <row r="188" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G188" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="189" spans="7:7">
+    <row r="189" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G189" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="190" spans="7:7">
+    <row r="190" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G190" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="191" spans="7:7">
+    <row r="191" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G191" s="2" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="192" spans="7:7">
+    <row r="192" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G192" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="193" spans="7:7">
+    <row r="193" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G193" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="194" spans="7:7">
+    <row r="194" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G194" s="2" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="195" spans="7:7">
+    <row r="195" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G195" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="196" spans="7:7">
+    <row r="196" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G196" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="197" spans="7:7">
+    <row r="197" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G197" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="198" spans="7:7">
+    <row r="198" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G198" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="199" spans="7:7">
+    <row r="199" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G199" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="200" spans="7:7">
+    <row r="200" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G200" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="201" spans="7:7">
+    <row r="201" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G201" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="202" spans="7:7">
+    <row r="202" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G202" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="203" spans="7:7">
+    <row r="203" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G203" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="204" spans="7:7">
+    <row r="204" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G204" s="2" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="205" spans="7:7">
+    <row r="205" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G205" s="2" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="206" spans="7:7">
+    <row r="206" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G206" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="207" spans="7:7">
+    <row r="207" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G207" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="208" spans="7:7">
+    <row r="208" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G208" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="209" spans="7:7">
+    <row r="209" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G209" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="210" spans="7:7">
+    <row r="210" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G210" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="211" spans="7:7">
+    <row r="211" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G211" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="212" spans="7:7">
+    <row r="212" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G212" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="213" spans="7:7">
+    <row r="213" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G213" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="214" spans="7:7">
+    <row r="214" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G214" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="215" spans="7:7">
+    <row r="215" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G215" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="216" spans="7:7">
+    <row r="216" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G216" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="217" spans="7:7">
+    <row r="217" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G217" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="218" spans="7:7">
+    <row r="218" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G218" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="219" spans="7:7">
+    <row r="219" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G219" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="220" spans="7:7">
+    <row r="220" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G220" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="221" spans="7:7">
+    <row r="221" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G221" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="222" spans="7:7">
+    <row r="222" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G222" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="223" spans="7:7">
+    <row r="223" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G223" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="224" spans="7:7">
+    <row r="224" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G224" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="225" spans="7:7">
+    <row r="225" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G225" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="226" spans="7:7">
+    <row r="226" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G226" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="227" spans="7:7">
+    <row r="227" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G227" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="228" spans="7:7">
+    <row r="228" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G228" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="229" spans="7:7">
+    <row r="229" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G229" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="230" spans="7:7">
+    <row r="230" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G230" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="231" spans="7:7">
+    <row r="231" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G231" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="232" spans="7:7">
+    <row r="232" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G232" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="233" spans="7:7">
+    <row r="233" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G233" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="234" spans="7:7">
+    <row r="234" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G234" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="235" spans="7:7">
+    <row r="235" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G235" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="236" spans="7:7">
+    <row r="236" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G236" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="237" spans="7:7">
+    <row r="237" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G237" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="238" spans="7:7">
+    <row r="238" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G238" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="239" spans="7:7">
+    <row r="239" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G239" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="240" spans="7:7">
+    <row r="240" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G240" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="241" spans="7:8">
+    <row r="241" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G241" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="242" spans="7:8">
+    <row r="242" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G242" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="243" spans="7:8">
+    <row r="243" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G243" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="244" spans="7:8">
+    <row r="244" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G244" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="245" spans="7:8">
+    <row r="245" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G245" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="246" spans="7:8">
+    <row r="246" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G246" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="247" spans="7:8">
+    <row r="247" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G247" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="248" spans="7:8">
+    <row r="248" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G248" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="249" spans="7:8">
+    <row r="249" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G249" s="2" t="s">
         <v>270</v>
       </c>
@@ -3989,288 +3995,288 @@
         <v>271</v>
       </c>
     </row>
-    <row r="250" spans="7:8">
+    <row r="250" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G250" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="251" spans="7:8">
+    <row r="251" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G251" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="252" spans="7:8">
+    <row r="252" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G252" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="253" spans="7:8">
+    <row r="253" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G253" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="254" spans="7:8">
+    <row r="254" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G254" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="255" spans="7:8">
+    <row r="255" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G255" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="256" spans="7:8">
+    <row r="256" spans="7:8" x14ac:dyDescent="0.15">
       <c r="G256" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="257" spans="7:7">
+    <row r="257" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G257" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="258" spans="7:7">
+    <row r="258" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G258" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="259" spans="7:7">
+    <row r="259" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G259" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="260" spans="7:7">
+    <row r="260" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G260" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="261" spans="7:7">
+    <row r="261" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G261" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="262" spans="7:7">
+    <row r="262" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G262" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="263" spans="7:7">
+    <row r="263" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G263" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="264" spans="7:7">
+    <row r="264" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G264" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="265" spans="7:7">
+    <row r="265" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G265" s="2" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="266" spans="7:7">
+    <row r="266" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G266" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="267" spans="7:7">
+    <row r="267" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G267" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="268" spans="7:7">
+    <row r="268" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G268" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="269" spans="7:7">
+    <row r="269" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G269" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="270" spans="7:7">
+    <row r="270" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G270" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="271" spans="7:7">
+    <row r="271" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G271" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="272" spans="7:7">
+    <row r="272" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G272" s="2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="273" spans="7:7">
+    <row r="273" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G273" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="274" spans="7:7">
+    <row r="274" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G274" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="275" spans="7:7">
+    <row r="275" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G275" s="2" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="276" spans="7:7">
+    <row r="276" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G276" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="277" spans="7:7">
+    <row r="277" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G277" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="278" spans="7:7">
+    <row r="278" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G278" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="279" spans="7:7">
+    <row r="279" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G279" s="2" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="280" spans="7:7">
+    <row r="280" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G280" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="281" spans="7:7">
+    <row r="281" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G281" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="282" spans="7:7">
+    <row r="282" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G282" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="283" spans="7:7">
+    <row r="283" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G283" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="284" spans="7:7">
+    <row r="284" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G284" s="2" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="285" spans="7:7">
+    <row r="285" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G285" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="286" spans="7:7">
+    <row r="286" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G286" s="2" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="287" spans="7:7">
+    <row r="287" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G287" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="288" spans="7:7">
+    <row r="288" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G288" s="2" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="289" spans="7:7">
+    <row r="289" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G289" s="2" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="290" spans="7:7">
+    <row r="290" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G290" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="291" spans="7:7">
+    <row r="291" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G291" s="2" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="292" spans="7:7">
+    <row r="292" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G292" s="2" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="293" spans="7:7">
+    <row r="293" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G293" s="2" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="294" spans="7:7">
+    <row r="294" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G294" s="2" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="295" spans="7:7">
+    <row r="295" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G295" s="2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="296" spans="7:7">
+    <row r="296" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G296" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="297" spans="7:7">
+    <row r="297" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G297" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="298" spans="7:7">
+    <row r="298" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G298" s="2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="299" spans="7:7">
+    <row r="299" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G299" s="2" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="300" spans="7:7">
+    <row r="300" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G300" s="2" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="301" spans="7:7">
+    <row r="301" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G301" s="2" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="302" spans="7:7">
+    <row r="302" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G302" s="2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="303" spans="7:7">
+    <row r="303" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G303" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="304" spans="7:7">
+    <row r="304" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G304" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="305" spans="7:7">
+    <row r="305" spans="7:7" x14ac:dyDescent="0.15">
       <c r="G305" s="2" t="s">
         <v>323</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H305">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H305">
     <sortCondition ref="G2:G305"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>